<commit_message>
update fdd, fds, odd vis logic
</commit_message>
<xml_diff>
--- a/FDD/test_output/Design_results.xlsx
+++ b/FDD/test_output/Design_results.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -521,36 +521,36 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>pntA_promoter_sub</t>
+          <t>aceE_del</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>CGAGGTTTGTGCCGTAAAGC</t>
+          <t>GCGTCACAGACATGAAATTGGT</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>AGGTATAATGCTAGCACGAATCTAGAGAAAGATTGGACGTACCATAATGCGAATTGGCATACCAAGAG</t>
+          <t>AGCCATTATTCTTTTACCTCGGGTTATTCCTTATCTATCT</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>CGAGGTTTGTGCCGTAAAGCTGTGAGGATTGCGTCGGCAGACGGCCCGGAAGATCGGTATAACCAATCACTTTGACACCATTTTCCGTAGTGAAGATTTCACCCGGCACGGTGTATTCACAGTTGCCGCCGTTTTGGGCTGCCAGGTCGACAATCACACTGCCCGCCTTCATGGAGTCAACCATTTCACGGGTAATTAGCTTCGGCGCTGGTTTGCCTGGAATAAGCGCGGTGGTGACAATGATATCGACCTCTTTTGCCTGGGCGGCAAAGAGTTCCATTTCCGCTTTGATGAACGCGTCCGACATCACTTTGGCATAGCCATCGCCGCTGCCAGCTTCCTCTTTAAAATCCAGCTCGAGGAATTCCGCGCCCATACTTTGAACTTGTTCTTTCACTTCCGGGCGGGTGTCGAATGCACGCACAATCGCGCCGAGACTGTTTGCTGCGCCAATGGCGGCCAGACCTGCAACACCCGCACCAATCACCATCACTTTTGCCGGTGGCACTTTCCCGGCCGCAGTAATTTGCCCGGTAAAGAAGCGCCCAAATTCATGTGCCGCTTCAACAATGGCGCGATAACCGGCGATGTTCGCCATCGAGCTTAGTGCGTCCAGCGATTGTGCGCGTGAGATACGCGGCACAGAGTCCATCGCCATCACGGTCACGTTACGTTCCGCAAGTTTTTGCATTAATTCCGGATTCTGCGCAGGCCAGATAAAACTCACCAGCGTTGTCCCAGGATTCAGTAACGCAATTTCATCATCTAACGGCGCATTGACCTTCAGAATGATCTCTGACTGCCAGACGCTATTCCCTTCTACAATTTCAGCGCCCGCTTGCACAAACGCTTTATCGTCAAAACTTGCCAGTTGACCCGCGCCGCTCTCTACCGCGACGGTAAAACCCAGTTTCAGCAGCTGTTCCACTGTTTTTGGCGTTGCTGCAACACGGGTTTCATTGGTTAACCGTTCTCTTGGTATGCCAATTCGCAT</t>
+          <t>GCGTCACAGACATGAAATTGGTAAGACCAATTGACTTCGGCAAGTGGCTTAAGACAGGAACTCATGGCCTACAGCAAAATCCGCCAACCAAAACTCTCCGATGTGATTGAGCAGCAACTGGAGTTTTTGATCCTCGAAGGCACTCTCCGCCCGGGCGAAAAACTCCCACCGGAACGCGAACTGGCAAAACAGTTTGACGTCTCCCGTCCCTCCTTGCGTGAGGCGATTCAACGTCTCGAAGCGAAGGGCTTGTTGCTTCGTCGCCAGGGTGGCGGCACTTTTGTCCAGAGCAGCCTATGGCAAAGCTTCAGCGATCCGCTGGTGGAGCTGCTCTCCGACCATCCTGAGTCACAGTATGACTTGCTCGAAACACGACACGCCCTGGAAGGTATCGCCGCTTATTACGCCGCGCTGCGTAGTACCGATGAAGACAAGGAACGCATCCGTGAACTCCACCACGCCATAGAGCTGGCGCAGCAGTCTGGCGATCTGGACGCGGAATCAAACGCCGTACTCCAGTATCAGATTGCCGTCACCGAAGCGGCCCACAATGTGGTTCTGCTTCATCTGCTAAGGTGTATGGAGCCGATGTTGGCCCAGAATGTCCGCCAGAACTTCGAATTGCTCTATTCGCGTCGCGAGATGCTGCCGCTGGTGAGTAGTCACCGCACCCGCATATTTGAAGCGATTATGGCCGGTAAGCCGGAAGAAGCGCGCGAAGCATCGCATCGCCATCTGGCCTTTATCGAAGAAATTTTGCTCGACAGAAGTCGTGAAGAGAGCCGCCGTGAGCGTTCTCTGCGTCGTCTGGAGCAACGAAAGAATTAGTGATTTTTCTGGTAAAAATTATCCAGAAGATGTTGTAAATCAAGCGCATATAAAAGCGCGGCAACTAAACGTAGAACCTGTCTTATTGAGCTTTCCGGCGAGAGTTCAATGGGACAGGTTCCAGAAAACTCAACGTTATTAGATAGATAAGGAATAACCC</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>ACCTGAATCGGCGGTGCCGGCCAGGTAATTTCGCCCGCACGGATCACGGTCACGCCGCGAATCACCACATCATCAAAATCAACAGTGATATTGCCGTCTTTCTCTTTGCACAACAGTTTCAGCAGATTAACGAGGTTTGTGCCGTAAAGCTGTGAGGATTGCGTCGGCAGACGGCCCGGAAGATCGGTATAACCAATCACTTTGACACCATTTTCCGTAGTGAAGATTTCACCCGGCACGGTGTATTCACAGTTGCCGCCGTTTTGGGCTGCCAGGTCGACAATCACACTGCCCGCCTTCATGGAGTCAACCATTTCACGGGTAATTAGCTTCGGCGCTGGTTTGCCTGGAATAAGCGCGGTGGTGACAATGATATCGACCTCTTTTGCCTGGGCGGCAAAGAGTTCCATTTCCGCTTTGATGAACGCGTCCGACATCACTTTGGCATAGCCATCGCCGCTGCCAGCTTCCTCTTTAAAATCCAGCTCGAGGAATTCCGCGCCCATACTTTGAACTTGTTCTTTCACTTCCGGGCGGGTGTCGAATGCACGCACAATCGCGCCGAGACTGTTTGCTGCGCCAATGGCGGCCAGACCTGCAACACCCGCACCAATCACCATCACTTTTGCCGGTGGCACTTTCCCGGCCGCAGTAATTTGCCCGGTAAAGAAGCGCCCAAATTCATGTGCCGCTTCAACAATGGCGCGATAACCGGCGATGTTCGCCATCGAGCTTAGTGCGTCCAGCGATTGTGCGCGTGAGATACGCGGCACAGAGTCCATCGCCATCACGGTCACGTTACGTTCCGCAAGTTTTTGCATTAATTCCGGATTCTGCGCAGGCCAGATAAAACTCACCAGCGTTGTCCCAGGATTCAGTAACGCAATTTCATCATCTAACGGCGCATTGACCTTCAGAATGATCTCTGACTGCCAGACGCTATTCCCTTCTACAATTTCAGCGCCCGCTTGCACAAACGCTTTATCGTCAAAACTTGCCAGTTGACCCGCGCCGCTCTCTACCGCGACGGTAAAACCCAGTTTCAGCAGCTGTTCCACTGTTTTTGGCGTTGCTGCAACACGGGTTTCATTGGTTAACCGTTCTCTTGGTATGCCAATTCGCAT</t>
+          <t>TACGTAAAGTCTACATTTGTGCATAGTTACAACTTTGAAACGTTATATATGTCAAGTTGTTAAAATGTGCACAGTTTCATGATTTCAATCAAAACCTGTATGGACATAAGGTGAATACTTTGTTACTTTAGCGTCACAGACATGAAATTGGTAAGACCAATTGACTTCGGCAAGTGGCTTAAGACAGGAACTCATGGCCTACAGCAAAATCCGCCAACCAAAACTCTCCGATGTGATTGAGCAGCAACTGGAGTTTTTGATCCTCGAAGGCACTCTCCGCCCGGGCGAAAAACTCCCACCGGAACGCGAACTGGCAAAACAGTTTGACGTCTCCCGTCCCTCCTTGCGTGAGGCGATTCAACGTCTCGAAGCGAAGGGCTTGTTGCTTCGTCGCCAGGGTGGCGGCACTTTTGTCCAGAGCAGCCTATGGCAAAGCTTCAGCGATCCGCTGGTGGAGCTGCTCTCCGACCATCCTGAGTCACAGTATGACTTGCTCGAAACACGACACGCCCTGGAAGGTATCGCCGCTTATTACGCCGCGCTGCGTAGTACCGATGAAGACAAGGAACGCATCCGTGAACTCCACCACGCCATAGAGCTGGCGCAGCAGTCTGGCGATCTGGACGCGGAATCAAACGCCGTACTCCAGTATCAGATTGCCGTCACCGAAGCGGCCCACAATGTGGTTCTGCTTCATCTGCTAAGGTGTATGGAGCCGATGTTGGCCCAGAATGTCCGCCAGAACTTCGAATTGCTCTATTCGCGTCGCGAGATGCTGCCGCTGGTGAGTAGTCACCGCACCCGCATATTTGAAGCGATTATGGCCGGTAAGCCGGAAGAAGCGCGCGAAGCATCGCATCGCCATCTGGCCTTTATCGAAGAAATTTTGCTCGACAGAAGTCGTGAAGAGAGCCGCCGTGAGCGTTCTCTGCGTCGTCTGGAGCAACGAAAGAATTAGTGATTTTTCTGGTAAAAATTATCCAGAAGATGTTGTAAATCAAGCGCATATAAAAGCGCGGCAACTAAACGTAGAACCTGTCTTATTGAGCTTTCCGGCGAGAGTTCAATGGGACAGGTTCCAGAAAACTCAACGTTATTAGATAGATAAGGAATAACCC</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>CGAGGTTTGTGCCGTAAAGCTGTGAGGATTGCGTCGGCAGACGGCCCGGAAGATCGGTATAACCAATCACTTTGACACCATTTTCCGTAGTGAAGATTTCACCCGGCACGGTGTATTCACAGTTGCCGCCGTTTTGGGCTGCCAGGTCGACAATCACACTGCCCGCCTTCATGGAGTCAACCATTTCACGGGTAATTAGCTTCGGCGCTGGTTTGCCTGGAATAAGCGCGGTGGTGACAATGATATCGACCTCTTTTGCCTGGGCGGCAAAGAGTTCCATTTCCGCTTTGATGAACGCGTCCGACATCACTTTGGCATAGCCATCGCCGCTGCCAGCTTCCTCTTTAAAATCCAGCTCGAGGAATTCCGCGCCCATACTTTGAACTTGTTCTTTCACTTCCGGGCGGGTGTCGAATGCACGCACAATCGCGCCGAGACTGTTTGCTGCGCCAATGGCGGCCAGACCTGCAACACCCGCACCAATCACCATCACTTTTGCCGGTGGCACTTTCCCGGCCGCAGTAATTTGCCCGGTAAAGAAGCGCCCAAATTCATGTGCCGCTTCAACAATGGCGCGATAACCGGCGATGTTCGCCATCGAGCTTAGTGCGTCCAGCGATTGTGCGCGTGAGATACGCGGCACAGAGTCCATCGCCATCACGGTCACGTTACGTTCCGCAAGTTTTTGCATTAATTCCGGATTCTGCGCAGGCCAGATAAAACTCACCAGCGTTGTCCCAGGATTCAGTAACGCAATTTCATCATCTAACGGCGCATTGACCTTCAGAATGATCTCTGACTGCCAGACGCTATTCCCTTCTACAATTTCAGCGCCCGCTTGCACAAACGCTTTATCGTCAAAACTTGCCAGTTGACCCGCGCCGCTCTCTACCGCGACGGTAAAACCCAGTTTCAGCAGCTGTTCCACTGTTTTTGGCGTTGCTGCAACACGGGTTTCATTGGTTAACCGTTCTCTTGGTATGCCAATTCGCATTATGGTACGTCCAATCTTTCTCTAGATTCGTGCTAGCATTATACCT</t>
+          <t>GCGTCACAGACATGAAATTGGTAAGACCAATTGACTTCGGCAAGTGGCTTAAGACAGGAACTCATGGCCTACAGCAAAATCCGCCAACCAAAACTCTCCGATGTGATTGAGCAGCAACTGGAGTTTTTGATCCTCGAAGGCACTCTCCGCCCGGGCGAAAAACTCCCACCGGAACGCGAACTGGCAAAACAGTTTGACGTCTCCCGTCCCTCCTTGCGTGAGGCGATTCAACGTCTCGAAGCGAAGGGCTTGTTGCTTCGTCGCCAGGGTGGCGGCACTTTTGTCCAGAGCAGCCTATGGCAAAGCTTCAGCGATCCGCTGGTGGAGCTGCTCTCCGACCATCCTGAGTCACAGTATGACTTGCTCGAAACACGACACGCCCTGGAAGGTATCGCCGCTTATTACGCCGCGCTGCGTAGTACCGATGAAGACAAGGAACGCATCCGTGAACTCCACCACGCCATAGAGCTGGCGCAGCAGTCTGGCGATCTGGACGCGGAATCAAACGCCGTACTCCAGTATCAGATTGCCGTCACCGAAGCGGCCCACAATGTGGTTCTGCTTCATCTGCTAAGGTGTATGGAGCCGATGTTGGCCCAGAATGTCCGCCAGAACTTCGAATTGCTCTATTCGCGTCGCGAGATGCTGCCGCTGGTGAGTAGTCACCGCACCCGCATATTTGAAGCGATTATGGCCGGTAAGCCGGAAGAAGCGCGCGAAGCATCGCATCGCCATCTGGCCTTTATCGAAGAAATTTTGCTCGACAGAAGTCGTGAAGAGAGCCGCCGTGAGCGTTCTCTGCGTCGTCTGGAGCAACGAAAGAATTAGTGATTTTTCTGGTAAAAATTATCCAGAAGATGTTGTAAATCAAGCGCATATAAAAGCGCGGCAACTAAACGTAGAACCTGTCTTATTGAGCTTTCCGGCGAGAGTTCAATGGGACAGGTTCCAGAAAACTCAACGTTATTAGATAGATAAGGAATAACCCGAGGTAAAAGAATAATGGCT</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>1040</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="4">
@@ -559,35 +559,73 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>pntA_promoter_sub</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>CGAGGTTTGTGCCGTAAAGC</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>AGGTATAATGCTAGCACGAATCTAGAGAAAGATTGGACGTACCATAATGCGAATTGGCATACCAAGAG</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>CGAGGTTTGTGCCGTAAAGCTGTGAGGATTGCGTCGGCAGACGGCCCGGAAGATCGGTATAACCAATCACTTTGACACCATTTTCCGTAGTGAAGATTTCACCCGGCACGGTGTATTCACAGTTGCCGCCGTTTTGGGCTGCCAGGTCGACAATCACACTGCCCGCCTTCATGGAGTCAACCATTTCACGGGTAATTAGCTTCGGCGCTGGTTTGCCTGGAATAAGCGCGGTGGTGACAATGATATCGACCTCTTTTGCCTGGGCGGCAAAGAGTTCCATTTCCGCTTTGATGAACGCGTCCGACATCACTTTGGCATAGCCATCGCCGCTGCCAGCTTCCTCTTTAAAATCCAGCTCGAGGAATTCCGCGCCCATACTTTGAACTTGTTCTTTCACTTCCGGGCGGGTGTCGAATGCACGCACAATCGCGCCGAGACTGTTTGCTGCGCCAATGGCGGCCAGACCTGCAACACCCGCACCAATCACCATCACTTTTGCCGGTGGCACTTTCCCGGCCGCAGTAATTTGCCCGGTAAAGAAGCGCCCAAATTCATGTGCCGCTTCAACAATGGCGCGATAACCGGCGATGTTCGCCATCGAGCTTAGTGCGTCCAGCGATTGTGCGCGTGAGATACGCGGCACAGAGTCCATCGCCATCACGGTCACGTTACGTTCCGCAAGTTTTTGCATTAATTCCGGATTCTGCGCAGGCCAGATAAAACTCACCAGCGTTGTCCCAGGATTCAGTAACGCAATTTCATCATCTAACGGCGCATTGACCTTCAGAATGATCTCTGACTGCCAGACGCTATTCCCTTCTACAATTTCAGCGCCCGCTTGCACAAACGCTTTATCGTCAAAACTTGCCAGTTGACCCGCGCCGCTCTCTACCGCGACGGTAAAACCCAGTTTCAGCAGCTGTTCCACTGTTTTTGGCGTTGCTGCAACACGGGTTTCATTGGTTAACCGTTCTCTTGGTATGCCAATTCGCAT</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>ACCTGAATCGGCGGTGCCGGCCAGGTAATTTCGCCCGCACGGATCACGGTCACGCCGCGAATCACCACATCATCAAAATCAACAGTGATATTGCCGTCTTTCTCTTTGCACAACAGTTTCAGCAGATTAACGAGGTTTGTGCCGTAAAGCTGTGAGGATTGCGTCGGCAGACGGCCCGGAAGATCGGTATAACCAATCACTTTGACACCATTTTCCGTAGTGAAGATTTCACCCGGCACGGTGTATTCACAGTTGCCGCCGTTTTGGGCTGCCAGGTCGACAATCACACTGCCCGCCTTCATGGAGTCAACCATTTCACGGGTAATTAGCTTCGGCGCTGGTTTGCCTGGAATAAGCGCGGTGGTGACAATGATATCGACCTCTTTTGCCTGGGCGGCAAAGAGTTCCATTTCCGCTTTGATGAACGCGTCCGACATCACTTTGGCATAGCCATCGCCGCTGCCAGCTTCCTCTTTAAAATCCAGCTCGAGGAATTCCGCGCCCATACTTTGAACTTGTTCTTTCACTTCCGGGCGGGTGTCGAATGCACGCACAATCGCGCCGAGACTGTTTGCTGCGCCAATGGCGGCCAGACCTGCAACACCCGCACCAATCACCATCACTTTTGCCGGTGGCACTTTCCCGGCCGCAGTAATTTGCCCGGTAAAGAAGCGCCCAAATTCATGTGCCGCTTCAACAATGGCGCGATAACCGGCGATGTTCGCCATCGAGCTTAGTGCGTCCAGCGATTGTGCGCGTGAGATACGCGGCACAGAGTCCATCGCCATCACGGTCACGTTACGTTCCGCAAGTTTTTGCATTAATTCCGGATTCTGCGCAGGCCAGATAAAACTCACCAGCGTTGTCCCAGGATTCAGTAACGCAATTTCATCATCTAACGGCGCATTGACCTTCAGAATGATCTCTGACTGCCAGACGCTATTCCCTTCTACAATTTCAGCGCCCGCTTGCACAAACGCTTTATCGTCAAAACTTGCCAGTTGACCCGCGCCGCTCTCTACCGCGACGGTAAAACCCAGTTTCAGCAGCTGTTCCACTGTTTTTGGCGTTGCTGCAACACGGGTTTCATTGGTTAACCGTTCTCTTGGTATGCCAATTCGCAT</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>CGAGGTTTGTGCCGTAAAGCTGTGAGGATTGCGTCGGCAGACGGCCCGGAAGATCGGTATAACCAATCACTTTGACACCATTTTCCGTAGTGAAGATTTCACCCGGCACGGTGTATTCACAGTTGCCGCCGTTTTGGGCTGCCAGGTCGACAATCACACTGCCCGCCTTCATGGAGTCAACCATTTCACGGGTAATTAGCTTCGGCGCTGGTTTGCCTGGAATAAGCGCGGTGGTGACAATGATATCGACCTCTTTTGCCTGGGCGGCAAAGAGTTCCATTTCCGCTTTGATGAACGCGTCCGACATCACTTTGGCATAGCCATCGCCGCTGCCAGCTTCCTCTTTAAAATCCAGCTCGAGGAATTCCGCGCCCATACTTTGAACTTGTTCTTTCACTTCCGGGCGGGTGTCGAATGCACGCACAATCGCGCCGAGACTGTTTGCTGCGCCAATGGCGGCCAGACCTGCAACACCCGCACCAATCACCATCACTTTTGCCGGTGGCACTTTCCCGGCCGCAGTAATTTGCCCGGTAAAGAAGCGCCCAAATTCATGTGCCGCTTCAACAATGGCGCGATAACCGGCGATGTTCGCCATCGAGCTTAGTGCGTCCAGCGATTGTGCGCGTGAGATACGCGGCACAGAGTCCATCGCCATCACGGTCACGTTACGTTCCGCAAGTTTTTGCATTAATTCCGGATTCTGCGCAGGCCAGATAAAACTCACCAGCGTTGTCCCAGGATTCAGTAACGCAATTTCATCATCTAACGGCGCATTGACCTTCAGAATGATCTCTGACTGCCAGACGCTATTCCCTTCTACAATTTCAGCGCCCGCTTGCACAAACGCTTTATCGTCAAAACTTGCCAGTTGACCCGCGCCGCTCTCTACCGCGACGGTAAAACCCAGTTTCAGCAGCTGTTCCACTGTTTTTGGCGTTGCTGCAACACGGGTTTCATTGGTTAACCGTTCTCTTGGTATGCCAATTCGCATTATGGTACGTCCAATCTTTCTCTAGATTCGTGCTAGCATTATACCT</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>Cgl1452_ins</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>CACTGCGCGGGATTTTATGG</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>TCAATACTCTTTTTGGCGCGCATGTGAACGCCTGACCAGG</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>CACTGCGCGGGATTTTATGGAGATTCACTTACCTAAAGATTTACGTGAACTGTGCGATCTCGATAGCTTAAAACTGGAATCCGCCAGCTTTGTCGATGAAAAATTGCGGGCGCTACACTCCGATATTTTATGGTCGGTAAAGACCCGCGAAGGCGATGGCTATATCTATGTGGTGATTGAACATCAGAGCCGCGAGGACATTCATATGGCCTTTCGCCTGATGCGCTATTCCATGGCGGTGATGTAGCGCCATATAGAGCATGATAAACGCCAGCCGCTACCGTTGGTCATCCCGATGCTATTTTATCACGGTAGCCGTAGTCCTTACCCCTGGTCCCTGTGCTGGCTGGACGAATTTGCCGACCCGACTACCGCACGGAAGCTTTATAACGCCGCGTTCCCGCTGGTGGATGTTACTGTCGTGCCAGACGACGAGATTGTGCAGCATCGCAGAGTCGCCCTGTTGGAGTTGATCCAAAAGCATATTCGCCAGCGCGATCTGATGGGGCTTATCGATCAACTGGTAGTATTACTGGTTACAGAGTGTGCTAATGACAGCCAGATAACTGCGCTGTTAAATTACATTTTACTGACTGGCGATGAAGCGCGTTTTAATGAGTTTATCAGTGAACTTACCCGTCGAATGCCACAACACAGGGAGCGAATAATGACGATTGCAGAGCGAATTCATAATGATGGATATATAAAAGGGGAGCAGCGCATTCTTCGATTGTTGTTGCAGAATGGGGCGGATCCTGAATGGATACAAAAGATTACCGGACTTTCGGCAGAGCAAATGCAGGCATTAAGGCAGCCCTTGCCTGAGCGTGAGCGCTATTCATGGCTCAAGAGCTAATCAGAGACGGATGACAAACGCAAAGCAGCCTGATGCGCTATGCTTATCAGGTCTACATAACCCATTAAATATATTGAACTTTAAAGATTTTTGTAGACCTGGTCAGGCGTTCACATG</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>CGGGTGAGAATGGTTTTGTTAGTCGCTAAAGTCAGGCCATCTTTTTCAACAGGTGATGGATCGCCATGACAAACTTCACGACCAGCACGCCGCATGATGCATTATTTAAAACCTTTCTCACGCACCCTGACACTGCGCGGGATTTTATGGAGATTCACTTACCTAAAGATTTACGTGAACTGTGCGATCTCGATAGCTTAAAACTGGAATCCGCCAGCTTTGTCGATGAAAAATTGCGGGCGCTACACTCCGATATTTTATGGTCGGTAAAGACCCGCGAAGGCGATGGCTATATCTATGTGGTGATTGAACATCAGAGCCGCGAGGACATTCATATGGCCTTTCGCCTGATGCGCTATTCCATGGCGGTGATGTAGCGCCATATAGAGCATGATAAACGCCAGCCGCTACCGTTGGTCATCCCGATGCTATTTTATCACGGTAGCCGTAGTCCTTACCCCTGGTCCCTGTGCTGGCTGGACGAATTTGCCGACCCGACTACCGCACGGAAGCTTTATAACGCCGCGTTCCCGCTGGTGGATGTTACTGTCGTGCCAGACGACGAGATTGTGCAGCATCGCAGAGTCGCCCTGTTGGAGTTGATCCAAAAGCATATTCGCCAGCGCGATCTGATGGGGCTTATCGATCAACTGGTAGTATTACTGGTTACAGAGTGTGCTAATGACAGCCAGATAACTGCGCTGTTAAATTACATTTTACTGACTGGCGATGAAGCGCGTTTTAATGAGTTTATCAGTGAACTTACCCGTCGAATGCCACAACACAGGGAGCGAATAATGACGATTGCAGAGCGAATTCATAATGATGGATATATAAAAGGGGAGCAGCGCATTCTTCGATTGTTGTTGCAGAATGGGGCGGATCCTGAATGGATACAAAAGATTACCGGACTTTCGGCAGAGCAAATGCAGGCATTAAGGCAGCCCTTGCCTGAGCGTGAGCGCTATTCATGGCTCAAGAGCTAATCAGAGACGGATGACAAACGCAAAGCAGCCTGATGCGCTATGCTTATCAGGTCTACATAACCCATTAAATATATTGAACTTTAAAGATTTTTGTAGACCTGGTCAGGCGTTCACATG</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>CACTGCGCGGGATTTTATGGAGATTCACTTACCTAAAGATTTACGTGAACTGTGCGATCTCGATAGCTTAAAACTGGAATCCGCCAGCTTTGTCGATGAAAAATTGCGGGCGCTACACTCCGATATTTTATGGTCGGTAAAGACCCGCGAAGGCGATGGCTATATCTATGTGGTGATTGAACATCAGAGCCGCGAGGACATTCATATGGCCTTTCGCCTGATGCGCTATTCCATGGCGGTGATGTAGCGCCATATAGAGCATGATAAACGCCAGCCGCTACCGTTGGTCATCCCGATGCTATTTTATCACGGTAGCCGTAGTCCTTACCCCTGGTCCCTGTGCTGGCTGGACGAATTTGCCGACCCGACTACCGCACGGAAGCTTTATAACGCCGCGTTCCCGCTGGTGGATGTTACTGTCGTGCCAGACGACGAGATTGTGCAGCATCGCAGAGTCGCCCTGTTGGAGTTGATCCAAAAGCATATTCGCCAGCGCGATCTGATGGGGCTTATCGATCAACTGGTAGTATTACTGGTTACAGAGTGTGCTAATGACAGCCAGATAACTGCGCTGTTAAATTACATTTTACTGACTGGCGATGAAGCGCGTTTTAATGAGTTTATCAGTGAACTTACCCGTCGAATGCCACAACACAGGGAGCGAATAATGACGATTGCAGAGCGAATTCATAATGATGGATATATAAAAGGGGAGCAGCGCATTCTTCGATTGTTGTTGCAGAATGGGGCGGATCCTGAATGGATACAAAAGATTACCGGACTTTCGGCAGAGCAAATGCAGGCATTAAGGCAGCCCTTGCCTGAGCGTGAGCGCTATTCATGGCTCAAGAGCTAATCAGAGACGGATGACAAACGCAAAGCAGCCTGATGCGCTATGCTTATCAGGTCTACATAACCCATTAAATATATTGAACTTTAAAGATTTTTGTAGACCTGGTCAGGCGTTCACATGCGCGCCAAAAAGAGTATTGA</t>
         </is>
       </c>
-      <c r="H4" t="n">
+      <c r="H5" t="n">
         <v>993</v>
       </c>
     </row>
@@ -602,7 +640,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -691,35 +729,35 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>pntA_promoter_sub</t>
+          <t>aceE_del</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>TTCGTGCTAGCATTATACCTAGGACTGAGCTAGCTGTCAAGGCGCGGTGATAGTGGGATAAACACCT</t>
+          <t>GAGGTAAAAGAATAATGGCTATCGA</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>ACTTGGTGATGCGGTAGTCG</t>
+          <t>TTAACACCAAACTCGCGTGC</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>TTCGTGCTAGCATTATACCTAGGACTGAGCTAGCTGTCAAGGCGCGGTGATAGTGGGATAAACACCTTAGAACGCCGGATAAAGACTGATAATTGTCTTCGACGGTCGGGTAAAACGAGACATCGCCCCGGCACGAATCACTACTTAACATTAAATTAACTTATACAATTCAGTTGCTTCAGTAGTAATGATGCTGATACGGCTGTTTTTTAAGCATAGACGGTCATTTGAGCAGGATTAAAATTGGCTTAAGGAATGTGATATGAAAAATGACGCAGACAGTTACACCGTTTAAATGCAATAATCAGCCACGTTTCTCGTTAATAACAATACCAGTACCTGGTTTGCGCAAGGCGAAGGATTATTTTTATGAAGCTTAAGAACACCCTCCTGGCGTCGGCACTGCTTTCTGCTATGGCATTCTCCGTTAACGCAGCAACAGAACTGACACCGGAGCAAGCGGCAGCGGTTAAACCTTTTGACCGTGTAGTGGTTACCGGTCGTTTTAATGCTATTGGCGAAGCGGTGAAAGCCGTTTCTCGTCGCGCAGATAAAGAAGGTGCCGCCTCTTTTTATGTTGTCGACACTTCTGATTTTGGTAACAGCGGTAACTGGCGTGTGGTCGCTGACCTCTATAAAGCCGATGCTGAAAAAGCAGAAGAAACAAGTAATCGCGTAATTAACGGTGTTGTCGAACTGCCGAAAGATCAGGCTGTTCTGATTGAACCGTTTGACACGGTCACCGTCCAGGGCTTCTATCGTAGCCAGCCAGAAGTCAATGATGCCATCACCAAAGCGGCAAAAGCGAAAGGTGCCTACTCTTTCTACATCGTTCGTCAAATCGATGCCAACCAGGGCGGCAACCAGCGTATTACTGCATTCATCTATAAAAAAGATGCTAAGAAACGTATCGTCCAGAGCCCGGATGTGATCCCGGCAGATTCCGAAGCAGGACGTGCAGCTCTGGCTGCCGGTGGCGAAGCCGCGAAGAAAGTTGAGATCCCGGGTGTTGCGACTACCGCATCACCAAGT</t>
+          <t>GAGGTAAAAGAATAATGGCTATCGAAATCAAAGTACCGGACATCGGGGCTGATGAAGTTGAAATCACCGAGATCCTGGTCAAAGTGGGCGACAAAGTTGAAGCCGAACAGTCGCTGATCACCGTAGAAGGCGACAAAGCCTCTATGGAAGTTCCGTCTCCGCAGGCGGGTATCGTTAAAGAGATCAAAGTCTCTGTTGGCGATAAAACCCAGACCGGCGCACTGATTATGATTTTCGATTCCGCCGACGGTGCAGCAGACGCTGCACCTGCTCAGGCAGAAGAGAAGAAAGAAGCAGCTCCGGCAGCAGCACCAGCGGCTGCGGCGGCAAAAGACGTTAACGTTCCGGATATCGGCAGCGACGAAGTTGAAGTGACCGAAATCCTGGTGAAAGTTGGCGATAAAGTTGAAGCTGAACAGTCGCTGATCACCGTAGAAGGCGACAAGGCTTCTATGGAAGTTCCGGCTCCGTTTGCTGGCACCGTGAAAGAGATCAAAGTGAACGTGGGTGACAAAGTGTCTACCGGCTCGCTGATTATGGTCTTCGAAGTCGCGGGTGAAGCAGGCGCGGCAGCTCCGGCCGCTAAACAGGAAGCAGCTCCGGCAGCGGCCCCTGCACCAGCGGCTGGCGTGAAAGAAGTTAACGTTCCGGATATCGGCGGTGACGAAGTTGAAGTGACTGAAGTGATGGTGAAAGTGGGCGACAAAGTTGCCGCTGAACAGTCACTGATCACCGTAGAAGGCGACAAAGCTTCTATGGAAGTTCCGGCGCCGTTTGCAGGCGTCGTGAAGGAACTGAAAGTCAACGTTGGCGATAAAGTGAAAACTGGCTCGCTGATTATGATCTTCGAAGTTGAAGGCGCAGCGCCTGCGGCAGCTCCTGCGAAACAGGAAGCGGCAGCGCCGGCACCGGCAGCAAAAGCTGAAGCCCCGGCAGCAGCACCAGCTGCGAAAGCGGAAGGCAAATCTGAATTTGCTGAAAACGACGCTTATGTTCACGCGACTCCGCTGATCCGCCGTCTGGCACGCGAGTTTGGTGTTAA</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>1032</v>
+        <v>1042</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>GTGATAGTGGGATAAACACCTTAGAACGCCGGATAAAGACTGATAATTGTCTTCGACGGTCGGGTAAAACGAGACATCGCCCCGGCACGAATCACTACTTAACATTAAATTAACTTATACAATTCAGTTGCTTCAGTAGTAATGATGCTGATACGGCTGTTTTTTAAGCATAGACGGTCATTTGAGCAGGATTAAAATTGGCTTAAGGAATGTGATATGAAAAATGACGCAGACAGTTACACCGTTTAAATGCAATAATCAGCCACGTTTCTCGTTAATAACAATACCAGTACCTGGTTTGCGCAAGGCGAAGGATTATTTTTATGAAGCTTAAGAACACCCTCCTGGCGTCGGCACTGCTTTCTGCTATGGCATTCTCCGTTAACGCAGCAACAGAACTGACACCGGAGCAAGCGGCAGCGGTTAAACCTTTTGACCGTGTAGTGGTTACCGGTCGTTTTAATGCTATTGGCGAAGCGGTGAAAGCCGTTTCTCGTCGCGCAGATAAAGAAGGTGCCGCCTCTTTTTATGTTGTCGACACTTCTGATTTTGGTAACAGCGGTAACTGGCGTGTGGTCGCTGACCTCTATAAAGCCGATGCTGAAAAAGCAGAAGAAACAAGTAATCGCGTAATTAACGGTGTTGTCGAACTGCCGAAAGATCAGGCTGTTCTGATTGAACCGTTTGACACGGTCACCGTCCAGGGCTTCTATCGTAGCCAGCCAGAAGTCAATGATGCCATCACCAAAGCGGCAAAAGCGAAAGGTGCCTACTCTTTCTACATCGTTCGTCAAATCGATGCCAACCAGGGCGGCAACCAGCGTATTACTGCATTCATCTATAAAAAAGATGCTAAGAAACGTATCGTCCAGAGCCCGGATGTGATCCCGGCAGATTCCGAAGCAGGACGTGCAGCTCTGGCTGCCGGTGGCGAAGCCGCGAAGAAAGTTGAGATCCCGGGTGTTGCGACTACCGCATCACCAAGTTCTGAAGTCGGTCGCTTCTTTGAAACCCAGTCATCAAAAGGCGGGCGTTACACCGTCACGCTCCCGGATGGCACTAAAGTCGAAGAACTGAACAAAGCGACCGCAGCGATGATGGTCCCGTTCGACAGCA</t>
+          <t>GAGGTAAAAGAATAATGGCTATCGAAATCAAAGTACCGGACATCGGGGCTGATGAAGTTGAAATCACCGAGATCCTGGTCAAAGTGGGCGACAAAGTTGAAGCCGAACAGTCGCTGATCACCGTAGAAGGCGACAAAGCCTCTATGGAAGTTCCGTCTCCGCAGGCGGGTATCGTTAAAGAGATCAAAGTCTCTGTTGGCGATAAAACCCAGACCGGCGCACTGATTATGATTTTCGATTCCGCCGACGGTGCAGCAGACGCTGCACCTGCTCAGGCAGAAGAGAAGAAAGAAGCAGCTCCGGCAGCAGCACCAGCGGCTGCGGCGGCAAAAGACGTTAACGTTCCGGATATCGGCAGCGACGAAGTTGAAGTGACCGAAATCCTGGTGAAAGTTGGCGATAAAGTTGAAGCTGAACAGTCGCTGATCACCGTAGAAGGCGACAAGGCTTCTATGGAAGTTCCGGCTCCGTTTGCTGGCACCGTGAAAGAGATCAAAGTGAACGTGGGTGACAAAGTGTCTACCGGCTCGCTGATTATGGTCTTCGAAGTCGCGGGTGAAGCAGGCGCGGCAGCTCCGGCCGCTAAACAGGAAGCAGCTCCGGCAGCGGCCCCTGCACCAGCGGCTGGCGTGAAAGAAGTTAACGTTCCGGATATCGGCGGTGACGAAGTTGAAGTGACTGAAGTGATGGTGAAAGTGGGCGACAAAGTTGCCGCTGAACAGTCACTGATCACCGTAGAAGGCGACAAAGCTTCTATGGAAGTTCCGGCGCCGTTTGCAGGCGTCGTGAAGGAACTGAAAGTCAACGTTGGCGATAAAGTGAAAACTGGCTCGCTGATTATGATCTTCGAAGTTGAAGGCGCAGCGCCTGCGGCAGCTCCTGCGAAACAGGAAGCGGCAGCGCCGGCACCGGCAGCAAAAGCTGAAGCCCCGGCAGCAGCACCAGCTGCGAAAGCGGAAGGCAAATCTGAATTTGCTGAAAACGACGCTTATGTTCACGCGACTCCGCTGATCCGCCGTCTGGCACGCGAGTTTGGTGTTAACCTTGCGAAAGTGAAGGGCACTGGCCGTAAAGGTCGTATCCTGCGCGAAGACGTTCAGGCTTACGTGAAAGAAGCTATCAAACGTGCAGAAGCAGCTCCGGCAGCGACTGGCGGTGGTATCCCTGGCATG</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>GTGATAGTGGGATAAACACCTTAGAACGCCGGATAAAGACTGATAATTGTCTTCGACGGTCGGGTAAAACGAGACATCGCCCCGGCACGAATCACTACTTAACATTAAATTAACTTATACAATTCAGTTGCTTCAGTAGTAATGATGCTGATACGGCTGTTTTTTAAGCATAGACGGTCATTTGAGCAGGATTAAAATTGGCTTAAGGAATGTGATATGAAAAATGACGCAGACAGTTACACCGTTTAAATGCAATAATCAGCCACGTTTCTCGTTAATAACAATACCAGTACCTGGTTTGCGCAAGGCGAAGGATTATTTTTATGAAGCTTAAGAACACCCTCCTGGCGTCGGCACTGCTTTCTGCTATGGCATTCTCCGTTAACGCAGCAACAGAACTGACACCGGAGCAAGCGGCAGCGGTTAAACCTTTTGACCGTGTAGTGGTTACCGGTCGTTTTAATGCTATTGGCGAAGCGGTGAAAGCCGTTTCTCGTCGCGCAGATAAAGAAGGTGCCGCCTCTTTTTATGTTGTCGACACTTCTGATTTTGGTAACAGCGGTAACTGGCGTGTGGTCGCTGACCTCTATAAAGCCGATGCTGAAAAAGCAGAAGAAACAAGTAATCGCGTAATTAACGGTGTTGTCGAACTGCCGAAAGATCAGGCTGTTCTGATTGAACCGTTTGACACGGTCACCGTCCAGGGCTTCTATCGTAGCCAGCCAGAAGTCAATGATGCCATCACCAAAGCGGCAAAAGCGAAAGGTGCCTACTCTTTCTACATCGTTCGTCAAATCGATGCCAACCAGGGCGGCAACCAGCGTATTACTGCATTCATCTATAAAAAAGATGCTAAGAAACGTATCGTCCAGAGCCCGGATGTGATCCCGGCAGATTCCGAAGCAGGACGTGCAGCTCTGGCTGCCGGTGGCGAAGCCGCGAAGAAAGTTGAGATCCCGGGTGTTGCGACTACCGCATCACCAAGT</t>
+          <t>GAGGTAAAAGAATAATGGCTATCGAAATCAAAGTACCGGACATCGGGGCTGATGAAGTTGAAATCACCGAGATCCTGGTCAAAGTGGGCGACAAAGTTGAAGCCGAACAGTCGCTGATCACCGTAGAAGGCGACAAAGCCTCTATGGAAGTTCCGTCTCCGCAGGCGGGTATCGTTAAAGAGATCAAAGTCTCTGTTGGCGATAAAACCCAGACCGGCGCACTGATTATGATTTTCGATTCCGCCGACGGTGCAGCAGACGCTGCACCTGCTCAGGCAGAAGAGAAGAAAGAAGCAGCTCCGGCAGCAGCACCAGCGGCTGCGGCGGCAAAAGACGTTAACGTTCCGGATATCGGCAGCGACGAAGTTGAAGTGACCGAAATCCTGGTGAAAGTTGGCGATAAAGTTGAAGCTGAACAGTCGCTGATCACCGTAGAAGGCGACAAGGCTTCTATGGAAGTTCCGGCTCCGTTTGCTGGCACCGTGAAAGAGATCAAAGTGAACGTGGGTGACAAAGTGTCTACCGGCTCGCTGATTATGGTCTTCGAAGTCGCGGGTGAAGCAGGCGCGGCAGCTCCGGCCGCTAAACAGGAAGCAGCTCCGGCAGCGGCCCCTGCACCAGCGGCTGGCGTGAAAGAAGTTAACGTTCCGGATATCGGCGGTGACGAAGTTGAAGTGACTGAAGTGATGGTGAAAGTGGGCGACAAAGTTGCCGCTGAACAGTCACTGATCACCGTAGAAGGCGACAAAGCTTCTATGGAAGTTCCGGCGCCGTTTGCAGGCGTCGTGAAGGAACTGAAAGTCAACGTTGGCGATAAAGTGAAAACTGGCTCGCTGATTATGATCTTCGAAGTTGAAGGCGCAGCGCCTGCGGCAGCTCCTGCGAAACAGGAAGCGGCAGCGCCGGCACCGGCAGCAAAAGCTGAAGCCCCGGCAGCAGCACCAGCTGCGAAAGCGGAAGGCAAATCTGAATTTGCTGAAAACGACGCTTATGTTCACGCGACTCCGCTGATCCGCCGTCTGGCACGCGAGTTTGGTGTTAA</t>
         </is>
       </c>
     </row>
@@ -729,33 +767,71 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>pntA_promoter_sub</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>TTCGTGCTAGCATTATACCTAGGACTGAGCTAGCTGTCAAGGCGCGGTGATAGTGGGATAAACACCT</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>ACTTGGTGATGCGGTAGTCG</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>TTCGTGCTAGCATTATACCTAGGACTGAGCTAGCTGTCAAGGCGCGGTGATAGTGGGATAAACACCTTAGAACGCCGGATAAAGACTGATAATTGTCTTCGACGGTCGGGTAAAACGAGACATCGCCCCGGCACGAATCACTACTTAACATTAAATTAACTTATACAATTCAGTTGCTTCAGTAGTAATGATGCTGATACGGCTGTTTTTTAAGCATAGACGGTCATTTGAGCAGGATTAAAATTGGCTTAAGGAATGTGATATGAAAAATGACGCAGACAGTTACACCGTTTAAATGCAATAATCAGCCACGTTTCTCGTTAATAACAATACCAGTACCTGGTTTGCGCAAGGCGAAGGATTATTTTTATGAAGCTTAAGAACACCCTCCTGGCGTCGGCACTGCTTTCTGCTATGGCATTCTCCGTTAACGCAGCAACAGAACTGACACCGGAGCAAGCGGCAGCGGTTAAACCTTTTGACCGTGTAGTGGTTACCGGTCGTTTTAATGCTATTGGCGAAGCGGTGAAAGCCGTTTCTCGTCGCGCAGATAAAGAAGGTGCCGCCTCTTTTTATGTTGTCGACACTTCTGATTTTGGTAACAGCGGTAACTGGCGTGTGGTCGCTGACCTCTATAAAGCCGATGCTGAAAAAGCAGAAGAAACAAGTAATCGCGTAATTAACGGTGTTGTCGAACTGCCGAAAGATCAGGCTGTTCTGATTGAACCGTTTGACACGGTCACCGTCCAGGGCTTCTATCGTAGCCAGCCAGAAGTCAATGATGCCATCACCAAAGCGGCAAAAGCGAAAGGTGCCTACTCTTTCTACATCGTTCGTCAAATCGATGCCAACCAGGGCGGCAACCAGCGTATTACTGCATTCATCTATAAAAAAGATGCTAAGAAACGTATCGTCCAGAGCCCGGATGTGATCCCGGCAGATTCCGAAGCAGGACGTGCAGCTCTGGCTGCCGGTGGCGAAGCCGCGAAGAAAGTTGAGATCCCGGGTGTTGCGACTACCGCATCACCAAGT</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>1032</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>GTGATAGTGGGATAAACACCTTAGAACGCCGGATAAAGACTGATAATTGTCTTCGACGGTCGGGTAAAACGAGACATCGCCCCGGCACGAATCACTACTTAACATTAAATTAACTTATACAATTCAGTTGCTTCAGTAGTAATGATGCTGATACGGCTGTTTTTTAAGCATAGACGGTCATTTGAGCAGGATTAAAATTGGCTTAAGGAATGTGATATGAAAAATGACGCAGACAGTTACACCGTTTAAATGCAATAATCAGCCACGTTTCTCGTTAATAACAATACCAGTACCTGGTTTGCGCAAGGCGAAGGATTATTTTTATGAAGCTTAAGAACACCCTCCTGGCGTCGGCACTGCTTTCTGCTATGGCATTCTCCGTTAACGCAGCAACAGAACTGACACCGGAGCAAGCGGCAGCGGTTAAACCTTTTGACCGTGTAGTGGTTACCGGTCGTTTTAATGCTATTGGCGAAGCGGTGAAAGCCGTTTCTCGTCGCGCAGATAAAGAAGGTGCCGCCTCTTTTTATGTTGTCGACACTTCTGATTTTGGTAACAGCGGTAACTGGCGTGTGGTCGCTGACCTCTATAAAGCCGATGCTGAAAAAGCAGAAGAAACAAGTAATCGCGTAATTAACGGTGTTGTCGAACTGCCGAAAGATCAGGCTGTTCTGATTGAACCGTTTGACACGGTCACCGTCCAGGGCTTCTATCGTAGCCAGCCAGAAGTCAATGATGCCATCACCAAAGCGGCAAAAGCGAAAGGTGCCTACTCTTTCTACATCGTTCGTCAAATCGATGCCAACCAGGGCGGCAACCAGCGTATTACTGCATTCATCTATAAAAAAGATGCTAAGAAACGTATCGTCCAGAGCCCGGATGTGATCCCGGCAGATTCCGAAGCAGGACGTGCAGCTCTGGCTGCCGGTGGCGAAGCCGCGAAGAAAGTTGAGATCCCGGGTGTTGCGACTACCGCATCACCAAGTTCTGAAGTCGGTCGCTTCTTTGAAACCCAGTCATCAAAAGGCGGGCGTTACACCGTCACGCTCCCGGATGGCACTAAAGTCGAAGAACTGAACAAAGCGACCGCAGCGATGATGGTCCCGTTCGACAGCA</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>GTGATAGTGGGATAAACACCTTAGAACGCCGGATAAAGACTGATAATTGTCTTCGACGGTCGGGTAAAACGAGACATCGCCCCGGCACGAATCACTACTTAACATTAAATTAACTTATACAATTCAGTTGCTTCAGTAGTAATGATGCTGATACGGCTGTTTTTTAAGCATAGACGGTCATTTGAGCAGGATTAAAATTGGCTTAAGGAATGTGATATGAAAAATGACGCAGACAGTTACACCGTTTAAATGCAATAATCAGCCACGTTTCTCGTTAATAACAATACCAGTACCTGGTTTGCGCAAGGCGAAGGATTATTTTTATGAAGCTTAAGAACACCCTCCTGGCGTCGGCACTGCTTTCTGCTATGGCATTCTCCGTTAACGCAGCAACAGAACTGACACCGGAGCAAGCGGCAGCGGTTAAACCTTTTGACCGTGTAGTGGTTACCGGTCGTTTTAATGCTATTGGCGAAGCGGTGAAAGCCGTTTCTCGTCGCGCAGATAAAGAAGGTGCCGCCTCTTTTTATGTTGTCGACACTTCTGATTTTGGTAACAGCGGTAACTGGCGTGTGGTCGCTGACCTCTATAAAGCCGATGCTGAAAAAGCAGAAGAAACAAGTAATCGCGTAATTAACGGTGTTGTCGAACTGCCGAAAGATCAGGCTGTTCTGATTGAACCGTTTGACACGGTCACCGTCCAGGGCTTCTATCGTAGCCAGCCAGAAGTCAATGATGCCATCACCAAAGCGGCAAAAGCGAAAGGTGCCTACTCTTTCTACATCGTTCGTCAAATCGATGCCAACCAGGGCGGCAACCAGCGTATTACTGCATTCATCTATAAAAAAGATGCTAAGAAACGTATCGTCCAGAGCCCGGATGTGATCCCGGCAGATTCCGAAGCAGGACGTGCAGCTCTGGCTGCCGGTGGCGAAGCCGCGAAGAAAGTTGAGATCCCGGGTGTTGCGACTACCGCATCACCAAGT</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>Cgl1452_ins</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>GCTCCGAGGTTGAAGCTTAAGCATCCGGCATGAACAAAGC</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>CGATGTCGCTGGCGTTAATG</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>GCTCCGAGGTTGAAGCTTAAGCATCCGGCATGAACAAAGCGTACTTTGCTTAATTCAGGCTGGAACGTGGCGATGACCCAGCAAAGATAAAACGAGTCACAGGTTATGCATGAGAGGAAATCAGGCGCTTCGCCGCTATTTCGAATTTATTCCATTGCCCGATACACGGCCTCGCCAATTTGCTTCAGTGCTTCGCGATAGGTTTCGCTGAGCGGCAAAGCGCAGTTGATGCGCAGACAATTACGGTATTTGCCGGAAGCTGAGAAAATCGAGCCTGCCGCCACCTGGATTTTCATGCGGCACAGCTGCCGCGCGACGCAGACCATATCGACCTGTTCAGGCAATTCTATCCACAGTAAAAATCCGCCTTTCGGGCGCGTAATACAGATTTCGCAGGGAAAATATTCCCGTATCCAGCAGGTATAAAGCGCCAAATTGCGCTGATAGATCTGCCGCATCCGCCGGATATGGCGATGATAGTGACCTTCCAGCACAAACGTTGCCGCCGCCATTTGCGTGGACGGCACATTAAAGCTGCTGATGGCGTATTTCATATGCATCAGTTTATCGTGATAACGCCCCGGTGCGACCCAACCCACGCGCAGGCCTGGTGCAATACTTTTACTGAACGAGCTGCACAACAGCACTCGCCCGTCGATATCCCAGGAATGAATGGTCCGCGGGCGCGGATACTCCGTCGCCAGTTCGCCATAGACATCATCTTCAAAAATCACAATATCATGACGCTGAGCGAGAGAGAGAACGGCCCGTTTGCGCGCGTCCGGCATAATAAATCCCAGCGGATTATTACAGTTTGGCACCAGAATGATGCCTTTAATCGGCCACTGTTCCAGCGCCAGTTCCAGCGCTTCAACGCTGATGCCAGTTTCTGGATCGGTTGGGATTTCAATCACTTTCACGCCCATGCCGCGCAGCATCTGCATCGAACCGTAATAACAGGGGGATTCGACCGCGACAATATCGCCCGGTTTACACACTGCCATTAACGCCAGCGACATCG</t>
         </is>
       </c>
-      <c r="F4" t="n">
+      <c r="F5" t="n">
         <v>1021</v>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>GCATCCGGCATGAACAAAGCGTACTTTGCTTAATTCAGGCTGGAACGTGGCGATGACCCAGCAAAGATAAAACGAGTCACAGGTTATGCATGAGAGGAAATCAGGCGCTTCGCCGCTATTTCGAATTTATTCCATTGCCCGATACACGGCCTCGCCAATTTGCTTCAGTGCTTCGCGATAGGTTTCGCTGAGCGGCAAAGCGCAGTTGATGCGCAGACAATTACGGTATTTGCCGGAAGCTGAGAAAATCGAGCCTGCCGCCACCTGGATTTTCATGCGGCACAGCTGCCGCGCGACGCAGACCATATCGACCTGTTCAGGCAATTCTATCCACAGTAAAAATCCGCCTTTCGGGCGCGTAATACAGATTTCGCAGGGAAAATATTCCCGTATCCAGCAGGTATAAAGCGCCAAATTGCGCTGATAGATCTGCCGCATCCGCCGGATATGGCGATGATAGTGACCTTCCAGCACAAACGTTGCCGCCGCCATTTGCGTGGACGGCACATTAAAGCTGCTGATGGCGTATTTCATATGCATCAGTTTATCGTGATAACGCCCCGGTGCGACCCAACCCACGCGCAGGCCTGGTGCAATACTTTTACTGAACGAGCTGCACAACAGCACTCGCCCGTCGATATCCCAGGAATGAATGGTCCGCGGGCGCGGATACTCCGTCGCCAGTTCGCCATAGACATCATCTTCAAAAATCACAATATCATGACGCTGAGCGAGAGAGAGAACGGCCCGTTTGCGCGCGTCCGGCATAATAAATCCCAGCGGATTATTACAGTTTGGCACCAGAATGATGCCTTTAATCGGCCACTGTTCCAGCGCCAGTTCCAGCGCTTCAACGCTGATGCCAGTTTCTGGATCGGTTGGGATTTCAATCACTTTCACGCCCATGCCGCGCAGCATCTGCATCGAACCGTAATAACAGGGGGATTCGACCGCGACAATATCGCCCGGTTTACACACTGCCATTAACGCCAGCGACATCGAGTTATGGCAGCCGCTGGTGATGATGATGTCATCGGCGGTGACCACCGAGCCGCTGTCGAGCATCAGGCGGGCAATCTGCTCTCGCAATACTCGCTGACCGGCTAACAAGTCATAACCGAGAACGGTTTG</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>GCATCCGGCATGAACAAAGCGTACTTTGCTTAATTCAGGCTGGAACGTGGCGATGACCCAGCAAAGATAAAACGAGTCACAGGTTATGCATGAGAGGAAATCAGGCGCTTCGCCGCTATTTCGAATTTATTCCATTGCCCGATACACGGCCTCGCCAATTTGCTTCAGTGCTTCGCGATAGGTTTCGCTGAGCGGCAAAGCGCAGTTGATGCGCAGACAATTACGGTATTTGCCGGAAGCTGAGAAAATCGAGCCTGCCGCCACCTGGATTTTCATGCGGCACAGCTGCCGCGCGACGCAGACCATATCGACCTGTTCAGGCAATTCTATCCACAGTAAAAATCCGCCTTTCGGGCGCGTAATACAGATTTCGCAGGGAAAATATTCCCGTATCCAGCAGGTATAAAGCGCCAAATTGCGCTGATAGATCTGCCGCATCCGCCGGATATGGCGATGATAGTGACCTTCCAGCACAAACGTTGCCGCCGCCATTTGCGTGGACGGCACATTAAAGCTGCTGATGGCGTATTTCATATGCATCAGTTTATCGTGATAACGCCCCGGTGCGACCCAACCCACGCGCAGGCCTGGTGCAATACTTTTACTGAACGAGCTGCACAACAGCACTCGCCCGTCGATATCCCAGGAATGAATGGTCCGCGGGCGCGGATACTCCGTCGCCAGTTCGCCATAGACATCATCTTCAAAAATCACAATATCATGACGCTGAGCGAGAGAGAGAACGGCCCGTTTGCGCGCGTCCGGCATAATAAATCCCAGCGGATTATTACAGTTTGGCACCAGAATGATGCCTTTAATCGGCCACTGTTCCAGCGCCAGTTCCAGCGCTTCAACGCTGATGCCAGTTTCTGGATCGGTTGGGATTTCAATCACTTTCACGCCCATGCCGCGCAGCATCTGCATCGAACCGTAATAACAGGGGGATTCGACCGCGACAATATCGCCCGGTTTACACACTGCCATTAACGCCAGCGACATCG</t>
         </is>
@@ -1431,7 +1507,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1540,41 +1616,41 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>pntA_promoter_sub</t>
+          <t>aceE_del</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>TAATTTCGCCCGCACGGATCACGGTCACGCCGCGAATCACCACATCATCAAAATCAACAGTGATATTGCCGTCTTTCTCTTTGCACAACAGTTTCAGCAGATTAACGAGGTTTGTGCCGTAAAGCTGTGAGGATTGCGTCGGCAGACGGCCCGGAAGATCGGTATAACCAATCACTTTGACACCATTTTCCGTAGTGAAGATTTCACCCGGCACGGTGTATTCACAGTTGCCGCCGTTTTGGGCTGCCAGGTCGACAATCACACTGCCCGCCTTCATGGAGTCAACCATTTCACGGGTAATTAGCTTCGGCGCTGGTTTGCCTGGAATAAGCGCGGTGGTGACAATGATATCGACCTCTTTTGCCTGGGCGGCAAAGAGTTCCATTTCCGCTTTGATGAACGCGTCCGACATCACTTTGGCATAGCCATCGCCGCTGCCAGCTTCCTCTTTAAAATCCAGCTCGAGGAATTCCGCGCCCATACTTTGAACTTGTTCTTTCACTTCCGGGCGGGTGTCGAATGCACGCACAATCGCGCCGAGACTGTTTGCTGCGCCAATGGCGGCCAGACCTGCAACACCCGCACCAATCACCATCACTTTTGCCGGTGGCACTTTCCCGGCCGCAGTAATTTGCCCGGTAAAGAAGCGCCCAAATTCATGTGCCGCTTCAACAATGGCGCGATAACCGGCGATGTTCGCCATCGAGCTTAGTGCGTCCAGCGATTGTGCGCGTGAGATACGCGGCACAGAGTCCATCGCCATCACGGTCACGTTACGTTCCGCAAGTTTTTGCATTAATTCCGGATTCTGCGCAGGCCAGATAAAACTCACCAGCGTTGTCCCAGGATTCAGTAACGCAATTTCATCATCTAACGGCGCATTGACCTTCAGAATGATCTCTGACTGCCAGACGCTATTCCCTTCTACAATTTCAGCGCCCGCTTGCACAAACGCTTTATCGTCAAAACTTGCCAGTTGACCCGCGCCGCTCTCTACCGCGACGGTAAAACCCAGTTTCAGCAGCTGTTCCACTGTTTTTGGCGTTGCTGCAACACGGGTTTCATTGGTTAACCGTTCTCTTGGTATGCCAATTCGCATTATGGTACGTCCAATCTTTCTCTAGATTCGTGCTAGCATTATACCTAGGACTGAGCTAGCTGTCAAGGCGCGGTGATAGTGGGATAAACACCTTAGAACGCCGGATAAAGACTGATAATTGTCTTCGACGGTCGGGTAAAACGAGACATCGCCCCGGCACGAATCACTACTTAACATTAAATTAACTTATACAATTCAGTTGCTTCAGTAGTAATGATGCTGATACGGCTGTTTTTTAAGCATAGACGGTCATTTGAGCAGGATTAAAATTGGCTTAAGGAATGTGATATGAAAAATGACGCAGACAGTTACACCGTTTAAATGCAATAATCAGCCACGTTTCTCGTTAATAACAATACCAGTACCTGGTTTGCGCAAGGCGAAGGATTATTTTTATGAAGCTTAAGAACACCCTCCTGGCGTCGGCACTGCTTTCTGCTATGGCATTCTCCGTTAACGCAGCAACAGAACTGACACCGGAGCAAGCGGCAGCGGTTAAACCTTTTGACCGTGTAGTGGTTACCGGTCGTTTTAATGCTATTGGCGAAGCGGTGAAAGCCGTTTCTCGTCGCGCAGATAAAGAAGGTGCCGCCTCTTTTTATGTTGTCGACACTTCTGATTTTGGTAACAGCGGTAACTGGCGTGTGGTCGCTGACCTCTATAAAGCCGATGCTGAAAAAGCAGAAGAAACAAGTAATCGCGTAATTAACGGTGTTGTCGAACTGCCGAAAGATCAGGCTGTTCTGATTGAACCGTTTGACACGGTCACCGTCCAGGGCTTCTATCGTAGCCAGCCAGAAGTCAATGATGCCATCACCAAAGCGGCAAAAGCGAAAGGTGCCTACTCTTTCTACATCGTTCGTCAAATCGATGCCAACCAGGGCGGCAACCAGCGTATTACTGCATTCATCTATAAAAAAGATGCTAAGAAACGTATCGTCCAGAGCCCGGATGTGATCCCGGCAGATTCCGAAGCAGGACGTGCAGCTCTGGCTGCCGGTGGCGAAGCCGCGAAGAAAGTTGAGATCCCGGGTGTTGCGACTACCGCATCACCAAGTTCTGAAGTCGGTCGCTTCTTTGAAACCCAGTCATCAAAAGGCGGGCGTTACACCGTCACGCTCCCGGATGGCACTAAAGTCGAAGAACTGAACAAAGCGACCGCAGCGATGATGGTCCCGTTCGACA</t>
+          <t>ACGTAAAGTCTACATTTGTGCATAGTTACAACTTTGAAACGTTATATATGTCAAGTTGTTAAAATGTGCACAGTTTCATGATTTCAATCAAAACCTGTATGGACATAAGGTGAATACTTTGTTACTTTAGCGTCACAGACATGAAATTGGTAAGACCAATTGACTTCGGCAAGTGGCTTAAGACAGGAACTCATGGCCTACAGCAAAATCCGCCAACCAAAACTCTCCGATGTGATTGAGCAGCAACTGGAGTTTTTGATCCTCGAAGGCACTCTCCGCCCGGGCGAAAAACTCCCACCGGAACGCGAACTGGCAAAACAGTTTGACGTCTCCCGTCCCTCCTTGCGTGAGGCGATTCAACGTCTCGAAGCGAAGGGCTTGTTGCTTCGTCGCCAGGGTGGCGGCACTTTTGTCCAGAGCAGCCTATGGCAAAGCTTCAGCGATCCGCTGGTGGAGCTGCTCTCCGACCATCCTGAGTCACAGTATGACTTGCTCGAAACACGACACGCCCTGGAAGGTATCGCCGCTTATTACGCCGCGCTGCGTAGTACCGATGAAGACAAGGAACGCATCCGTGAACTCCACCACGCCATAGAGCTGGCGCAGCAGTCTGGCGATCTGGACGCGGAATCAAACGCCGTACTCCAGTATCAGATTGCCGTCACCGAAGCGGCCCACAATGTGGTTCTGCTTCATCTGCTAAGGTGTATGGAGCCGATGTTGGCCCAGAATGTCCGCCAGAACTTCGAATTGCTCTATTCGCGTCGCGAGATGCTGCCGCTGGTGAGTAGTCACCGCACCCGCATATTTGAAGCGATTATGGCCGGTAAGCCGGAAGAAGCGCGCGAAGCATCGCATCGCCATCTGGCCTTTATCGAAGAAATTTTGCTCGACAGAAGTCGTGAAGAGAGCCGCCGTGAGCGTTCTCTGCGTCGTCTGGAGCAACGAAAGAATTAGTGATTTTTCTGGTAAAAATTATCCAGAAGATGTTGTAAATCAAGCGCATATAAAAGCGCGGCAACTAAACGTAGAACCTGTCTTATTGAGCTTTCCGGCGAGAGTTCAATGGGACAGGTTCCAGAAAACTCAACGTTATTAGATAGATAAGGAATAACCCGAGGTAAAAGAATAATGGCTATCGAAATCAAAGTACCGGACATCGGGGCTGATGAAGTTGAAATCACCGAGATCCTGGTCAAAGTGGGCGACAAAGTTGAAGCCGAACAGTCGCTGATCACCGTAGAAGGCGACAAAGCCTCTATGGAAGTTCCGTCTCCGCAGGCGGGTATCGTTAAAGAGATCAAAGTCTCTGTTGGCGATAAAACCCAGACCGGCGCACTGATTATGATTTTCGATTCCGCCGACGGTGCAGCAGACGCTGCACCTGCTCAGGCAGAAGAGAAGAAAGAAGCAGCTCCGGCAGCAGCACCAGCGGCTGCGGCGGCAAAAGACGTTAACGTTCCGGATATCGGCAGCGACGAAGTTGAAGTGACCGAAATCCTGGTGAAAGTTGGCGATAAAGTTGAAGCTGAACAGTCGCTGATCACCGTAGAAGGCGACAAGGCTTCTATGGAAGTTCCGGCTCCGTTTGCTGGCACCGTGAAAGAGATCAAAGTGAACGTGGGTGACAAAGTGTCTACCGGCTCGCTGATTATGGTCTTCGAAGTCGCGGGTGAAGCAGGCGCGGCAGCTCCGGCCGCTAAACAGGAAGCAGCTCCGGCAGCGGCCCCTGCACCAGCGGCTGGCGTGAAAGAAGTTAACGTTCCGGATATCGGCGGTGACGAAGTTGAAGTGACTGAAGTGATGGTGAAAGTGGGCGACAAAGTTGCCGCTGAACAGTCACTGATCACCGTAGAAGGCGACAAAGCTTCTATGGAAGTTCCGGCGCCGTTTGCAGGCGTCGTGAAGGAACTGAAAGTCAACGTTGGCGATAAAGTGAAAACTGGCTCGCTGATTATGATCTTCGAAGTTGAAGGCGCAGCGCCTGCGGCAGCTCCTGCGAAACAGGAAGCGGCAGCGCCGGCACCGGCAGCAAAAGCTGAAGCCCCGGCAGCAGCACCAGCTGCGAAAGCGGAAGGCAAATCTGAATTTGCTGAAAACGACGCTTATGTTCACGCGACTCCGCTGATCCGCCGTCTGGCACGCGAGTTTGGTGTTAACCTTGCGAAAGTGAAGGGCACTGGCCGTAAAGGTCGTATCCTGCGCGAAGACGTTCAGGCTTACGTGAAAGAAGCTATCAAACGTGCAGAAGCAGCTCC</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>8.32323228564394</v>
+        <v>-42.60669801557233</v>
       </c>
       <c r="E3" t="n">
-        <v>-14.63116813722309</v>
+        <v>-0.900577242230667</v>
       </c>
       <c r="F3" t="n">
-        <v>10.99409519360194</v>
+        <v>-6.517879085020752</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>TAATTTCGCCCGCACGGAT</t>
+          <t>ACGTAAAGTCTACATTTGTGCA</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>TGTCGAACGGGACCATCATC</t>
+          <t>GGAGCTGCTTCTGCACGTTT</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>60.15332929800883</v>
+        <v>56.32043528895827</v>
       </c>
       <c r="J3" t="n">
-        <v>59.82515507935778</v>
+        <v>61.51048014864102</v>
       </c>
       <c r="K3" t="n">
-        <v>2284</v>
+        <v>2258</v>
       </c>
     </row>
     <row r="4">
@@ -1583,40 +1659,83 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>pntA_promoter_sub</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>TAATTTCGCCCGCACGGATCACGGTCACGCCGCGAATCACCACATCATCAAAATCAACAGTGATATTGCCGTCTTTCTCTTTGCACAACAGTTTCAGCAGATTAACGAGGTTTGTGCCGTAAAGCTGTGAGGATTGCGTCGGCAGACGGCCCGGAAGATCGGTATAACCAATCACTTTGACACCATTTTCCGTAGTGAAGATTTCACCCGGCACGGTGTATTCACAGTTGCCGCCGTTTTGGGCTGCCAGGTCGACAATCACACTGCCCGCCTTCATGGAGTCAACCATTTCACGGGTAATTAGCTTCGGCGCTGGTTTGCCTGGAATAAGCGCGGTGGTGACAATGATATCGACCTCTTTTGCCTGGGCGGCAAAGAGTTCCATTTCCGCTTTGATGAACGCGTCCGACATCACTTTGGCATAGCCATCGCCGCTGCCAGCTTCCTCTTTAAAATCCAGCTCGAGGAATTCCGCGCCCATACTTTGAACTTGTTCTTTCACTTCCGGGCGGGTGTCGAATGCACGCACAATCGCGCCGAGACTGTTTGCTGCGCCAATGGCGGCCAGACCTGCAACACCCGCACCAATCACCATCACTTTTGCCGGTGGCACTTTCCCGGCCGCAGTAATTTGCCCGGTAAAGAAGCGCCCAAATTCATGTGCCGCTTCAACAATGGCGCGATAACCGGCGATGTTCGCCATCGAGCTTAGTGCGTCCAGCGATTGTGCGCGTGAGATACGCGGCACAGAGTCCATCGCCATCACGGTCACGTTACGTTCCGCAAGTTTTTGCATTAATTCCGGATTCTGCGCAGGCCAGATAAAACTCACCAGCGTTGTCCCAGGATTCAGTAACGCAATTTCATCATCTAACGGCGCATTGACCTTCAGAATGATCTCTGACTGCCAGACGCTATTCCCTTCTACAATTTCAGCGCCCGCTTGCACAAACGCTTTATCGTCAAAACTTGCCAGTTGACCCGCGCCGCTCTCTACCGCGACGGTAAAACCCAGTTTCAGCAGCTGTTCCACTGTTTTTGGCGTTGCTGCAACACGGGTTTCATTGGTTAACCGTTCTCTTGGTATGCCAATTCGCATTATGGTACGTCCAATCTTTCTCTAGATTCGTGCTAGCATTATACCTAGGACTGAGCTAGCTGTCAAGGCGCGGTGATAGTGGGATAAACACCTTAGAACGCCGGATAAAGACTGATAATTGTCTTCGACGGTCGGGTAAAACGAGACATCGCCCCGGCACGAATCACTACTTAACATTAAATTAACTTATACAATTCAGTTGCTTCAGTAGTAATGATGCTGATACGGCTGTTTTTTAAGCATAGACGGTCATTTGAGCAGGATTAAAATTGGCTTAAGGAATGTGATATGAAAAATGACGCAGACAGTTACACCGTTTAAATGCAATAATCAGCCACGTTTCTCGTTAATAACAATACCAGTACCTGGTTTGCGCAAGGCGAAGGATTATTTTTATGAAGCTTAAGAACACCCTCCTGGCGTCGGCACTGCTTTCTGCTATGGCATTCTCCGTTAACGCAGCAACAGAACTGACACCGGAGCAAGCGGCAGCGGTTAAACCTTTTGACCGTGTAGTGGTTACCGGTCGTTTTAATGCTATTGGCGAAGCGGTGAAAGCCGTTTCTCGTCGCGCAGATAAAGAAGGTGCCGCCTCTTTTTATGTTGTCGACACTTCTGATTTTGGTAACAGCGGTAACTGGCGTGTGGTCGCTGACCTCTATAAAGCCGATGCTGAAAAAGCAGAAGAAACAAGTAATCGCGTAATTAACGGTGTTGTCGAACTGCCGAAAGATCAGGCTGTTCTGATTGAACCGTTTGACACGGTCACCGTCCAGGGCTTCTATCGTAGCCAGCCAGAAGTCAATGATGCCATCACCAAAGCGGCAAAAGCGAAAGGTGCCTACTCTTTCTACATCGTTCGTCAAATCGATGCCAACCAGGGCGGCAACCAGCGTATTACTGCATTCATCTATAAAAAAGATGCTAAGAAACGTATCGTCCAGAGCCCGGATGTGATCCCGGCAGATTCCGAAGCAGGACGTGCAGCTCTGGCTGCCGGTGGCGAAGCCGCGAAGAAAGTTGAGATCCCGGGTGTTGCGACTACCGCATCACCAAGTTCTGAAGTCGGTCGCTTCTTTGAAACCCAGTCATCAAAAGGCGGGCGTTACACCGTCACGCTCCCGGATGGCACTAAAGTCGAAGAACTGAACAAAGCGACCGCAGCGATGATGGTCCCGTTCGACA</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>8.32323228564394</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-14.63116813722309</v>
+      </c>
+      <c r="F4" t="n">
+        <v>10.99409519360194</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>TAATTTCGCCCGCACGGAT</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>TGTCGAACGGGACCATCATC</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>60.15332929800883</v>
+      </c>
+      <c r="J4" t="n">
+        <v>59.82515507935778</v>
+      </c>
+      <c r="K4" t="n">
+        <v>2284</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>Cgl1452_ins</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>AGTCGCTAAAGTCAGGCCATCTTTTTCAACAGGTGATGGATCGCCATGACAAACTTCACGACCAGCACGCCGCATGATGCATTATTTAAAACCTTTCTCACGCACCCTGACACTGCGCGGGATTTTATGGAGATTCACTTACCTAAAGATTTACGTGAACTGTGCGATCTCGATAGCTTAAAACTGGAATCCGCCAGCTTTGTCGATGAAAAATTGCGGGCGCTACACTCCGATATTTTATGGTCGGTAAAGACCCGCGAAGGCGATGGCTATATCTATGTGGTGATTGAACATCAGAGCCGCGAGGACATTCATATGGCCTTTCGCCTGATGCGCTATTCCATGGCGGTGATGTAGCGCCATATAGAGCATGATAAACGCCAGCCGCTACCGTTGGTCATCCCGATGCTATTTTATCACGGTAGCCGTAGTCCTTACCCCTGGTCCCTGTGCTGGCTGGACGAATTTGCCGACCCGACTACCGCACGGAAGCTTTATAACGCCGCGTTCCCGCTGGTGGATGTTACTGTCGTGCCAGACGACGAGATTGTGCAGCATCGCAGAGTCGCCCTGTTGGAGTTGATCCAAAAGCATATTCGCCAGCGCGATCTGATGGGGCTTATCGATCAACTGGTAGTATTACTGGTTACAGAGTGTGCTAATGACAGCCAGATAACTGCGCTGTTAAATTACATTTTACTGACTGGCGATGAAGCGCGTTTTAATGAGTTTATCAGTGAACTTACCCGTCGAATGCCACAACACAGGGAGCGAATAATGACGATTGCAGAGCGAATTCATAATGATGGATATATAAAAGGGGAGCAGCGCATTCTTCGATTGTTGTTGCAGAATGGGGCGGATCCTGAATGGATACAAAAGATTACCGGACTTTCGGCAGAGCAAATGCAGGCATTAAGGCAGCCCTTGCCTGAGCGTGAGCGCTATTCATGGCTCAAGAGCTAATCAGAGACGGATGACAAACGCAAAGCAGCCTGATGCGCTATGCTTATCAGGTCTACATAACCCATTAAATATATTGAACTTTAAAGATTTTTGTAGACCTGGTCAGGCGTTCACATGCGCGCCAAAAAGAGTATTGACTTCGCATCTTTTTGTACCCATAATTATTTCATTCACATCACACAGGAAAGGCCCATAATGCCGTCAAGTACGATCAATAACATGACTAATGGAGATAATCTCGCACAGATCGGCGTTGTAGGCCTAGCAGTAATGGGCTCAAACCTCGCCCGCAACTTCGCCCGCAACGGCAACACTGTCGCTGTCTACAACCGCAGCACTGACAAAACCGACAAGCTCATCGCCGATCACGGCTCCGAAGGCAACTTCATCCCTTCTGCAACCGTCGAAGAGTTCGTAGCATCCCTGGAAAAGCCACGCCGCGCCATCATCATGGTTCAGGCTGGTAACGCCACCGACGCAGTCATCAACCAGCTGGCAGATGCCATGGACGAAGGCGACATCATCATCGACGGCGGCAACGCCCTCTACACCGACACCATTCGTCGCGAGAAGGAAATCTCCGCACGCGGTCTCCACTTCGTCGGTGCTGGTATCTCCGGCGGCGAAGAAGGCGCACTCAACGGCCCATCCATCATGCCTGGTGGCCCAGCAAAGTCCTACGAGTCCCTCGGACCACTGCTTGAGTCCATCGCTGCCAACGTTGACGGCACCCCATGTGTCACCCACATCGGCCCAGACGGCGCCGGCCACTTCGTCAAGATGGTCCACAACGGCATCGAGTACGCCGACATGCAGGTCATCGGCGAGGCATACCACCTTCTCCGCTACGCAGCAGGCATGCAGCCAGCTGAAATCGCTGAGGTTTTCAAGGAATGGAACGCAGGCGACCTGGATTCCTACCTCATCGAAATCACCGCAGAGGTTCTCTCCCAGGTGGATGCTGAAACCGGCAAGCCACTAATCGACGTCATCGTTGACGCTGCAGGTCAGAAGGGCACCGGACGTTGGACCGTCAAGGCTGCTCTTGATCTGGGTATTGCTACCACCGGCATCGGCGAAGCTGTTTTCGCACGTGCACTCTCCGGCGCAACCAGCCAGCGCGCTGCAGCACAGGGCAACCTACCTGCAGGTGTCCTCACCGATCTGGAAGCACTTGGCGTGGACAAGGCACAGTTCGTCGAAGACGTTCGCCGTGCACTGTACGCATCCAAGCTTGTTGCTTACGCACAGGGCTTCGACGAGATCAAGGCTGGCTCCGACGAGAACAACTGGGACGTTGACCCTCGCGACCTCGCTACCATCTGGCGCGGCGGCTGCATCATTCGCGCTAAGTTCCTCAACCGCATCGTCGAAGCATACGATGCAAACGCTGAACTTGAGTCCCTGCTGCTCGATCCTTACTTCAAGAGCGAGCTCGGCGACCTCATCGATTCATGGCGTCGCGTGATTGTCACCGCCACCCAGCTTGGCCTGCCAATCCCAGTGTTCGCTTCCTCCCTGTCCTACTACGACAGCCTGCGTGCAGAGCGTCTGCCAGCAGCCCTGATCCAAGGACAGCGCGACTTCTTCGGTGCGCACACCTACAAGCGCATCGACAAGGATGGCTCCTTCCACACCGAGTGGTCCGGCGACCGCTCCGAGGTTGAAGCTTAAGCATCCGGCATGAACAAAGCGTACTTTGCTTAATTCAGGCTGGAACGTGGCGATGACCCAGCAAAGATAAAACGAGTCACAGGTTATGCATGAGAGGAAATCAGGCGCTTCGCCGCTATTTCGAATTTATTCCATTGCCCGATACACGGCCTCGCCAATTTGCTTCAGTGCTTCGCGATAGGTTTCGCTGAGCGGCAAAGCGCAGTTGATGCGCAGACAATTACGGTATTTGCCGGAAGCTGAGAAAATCGAGCCTGCCGCCACCTGGATTTTCATGCGGCACAGCTGCCGCGCGACGCAGACCATATCGACCTGTTCAGGCAATTCTATCCACAGTAAAAATCCGCCTTTCGGGCGCGTAATACAGATTTCGCAGGGAAAATATTCCCGTATCCAGCAGGTATAAAGCGCCAAATTGCGCTGATAGATCTGCCGCATCCGCCGGATATGGCGATGATAGTGACCTTCCAGCACAAACGTTGCCGCCGCCATTTGCGTGGACGGCACATTAAAGCTGCTGATGGCGTATTTCATATGCATCAGTTTATCGTGATAACGCCCCGGTGCGACCCAACCCACGCGCAGGCCTGGTGCAATACTTTTACTGAACGAGCTGCACAACAGCACTCGCCCGTCGATATCCCAGGAATGAATGGTCCGCGGGCGCGGATACTCCGTCGCCAGTTCGCCATAGACATCATCTTCAAAAATCACAATATCATGACGCTGAGCGAGAGAGAGAACGGCCCGTTTGCGCGCGTCCGGCATAATAAATCCCAGCGGATTATTACAGTTTGGCACCAGAATGATGCCTTTAATCGGCCACTGTTCCAGCGCCAGTTCCAGCGCTTCAACGCTGATGCCAGTTTCTGGATCGGTTGGGATTTCAATCACTTTCACGCCCATGCCGCGCAGCATCTGCATCGAACCGTAATAACAGGGGGATTCGACCGCGACAATATCGCCCGGTTTACACACTGCCATTAACGCCAGCGACATCGAGTTATGGCAGCCGCTGGTGATGATGATGTCATCGGCGGTGACCACCGAGCCGCTGTCGAGCATCAGGCGGGCAATCTGCTCTCGCAATACTCGCTGACCGGCTAACAAGTCA</t>
         </is>
       </c>
-      <c r="D4" t="n">
+      <c r="D5" t="n">
         <v>2.763999345539332</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E5" t="n">
         <v>-0.263335569570756</v>
       </c>
-      <c r="F4" t="n">
+      <c r="F5" t="n">
         <v>2.876222107101569</v>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>AGTCGCTAAAGTCAGGCCAT</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>TGACTTGTTAGCCGGTCAGC</t>
         </is>
       </c>
-      <c r="I4" t="n">
+      <c r="I5" t="n">
         <v>59.09464305682206</v>
       </c>
-      <c r="J4" t="n">
+      <c r="J5" t="n">
         <v>60.32042093038291</v>
       </c>
-      <c r="K4" t="n">
+      <c r="K5" t="n">
         <v>3754</v>
       </c>
     </row>

</xml_diff>